<commit_message>
Added feature skip awards as needed
</commit_message>
<xml_diff>
--- a/2025/2025-FLL-Qualifier-Tournaments.xlsx
+++ b/2025/2025-FLL-Qualifier-Tournaments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github-projects\OJS_Script_maker_NG\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2619415-C6C0-484F-8CA6-982B87C124A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71608BBE-1ED4-4A58-AA6A-C860F7D56834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0852510A-0402-494B-87EA-4B91755641F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0852510A-0402-494B-87EA-4B91755641F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
@@ -3081,148 +3081,148 @@
     <t>Unearthed</t>
   </si>
   <si>
-    <t>Newport News 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Henrico 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Glen Allen 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Martinsville 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Norfolk 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Blacksburg 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Abingdon 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Charlottesville 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Manassas 1 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Fairfax 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Manassas 2 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Richmond 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>DC-McKinley 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>DC-Friendship 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Ashburn 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>Alexandria 2025 Submerged Qualifier Tournament</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-newport_news-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-newport_news-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-henrico-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-henrico-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-glen_allen-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-glen_allen-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-martinsville-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-martinsville-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-norfolk-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-norfolk-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-blacksburg-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-blacksburg-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-abingdon-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-abingdon-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-charlottesville-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-charlottesville-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-manassas_1-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-fairfax-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-fairfax-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-manassas_2-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-richmond-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-richmond-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-dc-mckinley-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-dc-mckinley-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-dc-friendship-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-dc-friendship-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-ashburn-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-ashburn-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-alexandria-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-alexandria-div2.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-test-div1.xlsm</t>
-  </si>
-  <si>
-    <t>2025-vadc-fll-challenge-submerged-ojs-test-div2.xlsm</t>
+    <t>Newport News 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-newport_news-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-newport_news-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Henrico 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-henrico-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-henrico-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Glen Allen 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-glen_allen-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-glen_allen-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Martinsville 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-martinsville-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-martinsville-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Norfolk 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-norfolk-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-norfolk-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Blacksburg 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-blacksburg-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-blacksburg-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Abingdon 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-abingdon-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-abingdon-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Charlottesville 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-charlottesville-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-charlottesville-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Manassas 1 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-manassas_1-div1.xlsm</t>
+  </si>
+  <si>
+    <t>Fairfax 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-fairfax-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-fairfax-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Manassas 2 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-manassas_2-div1.xlsm</t>
+  </si>
+  <si>
+    <t>Richmond 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-richmond-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-richmond-div2.xlsm</t>
+  </si>
+  <si>
+    <t>DC-McKinley 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-dc-mckinley-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-dc-mckinley-div2.xlsm</t>
+  </si>
+  <si>
+    <t>DC-Friendship 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-dc-friendship-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-dc-friendship-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Ashburn 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-ashburn-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-ashburn-div2.xlsm</t>
+  </si>
+  <si>
+    <t>Alexandria 2025 Unearthed Qualifier Tournament</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-alexandria-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-alexandria-div2.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-test-div1.xlsm</t>
+  </si>
+  <si>
+    <t>2025-vadc-fll-challenge-Unearthed-ojs-test-div2.xlsm</t>
   </si>
 </sst>
 </file>
@@ -4490,7 +4490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F420C16-759B-4D97-9825-4887115BA2E4}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
@@ -5734,8 +5734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A41AF0E-5A5F-4597-97F4-A7EE3962C247}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5803,10 +5803,10 @@
         <v>45605</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1029</v>
+        <v>1014</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -5839,16 +5839,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="C3" s="2">
         <v>45605</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1031</v>
+        <v>1017</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1032</v>
+        <v>1018</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -5881,16 +5881,16 @@
         <v>649</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1015</v>
+        <v>1019</v>
       </c>
       <c r="C4" s="2">
         <v>45605</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1033</v>
+        <v>1020</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>1034</v>
+        <v>1021</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -5923,16 +5923,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1016</v>
+        <v>1022</v>
       </c>
       <c r="C5" s="2">
         <v>45605</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1035</v>
+        <v>1023</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1036</v>
+        <v>1024</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -5965,16 +5965,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1017</v>
+        <v>1025</v>
       </c>
       <c r="C6" s="2">
         <v>45612</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1037</v>
+        <v>1026</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1038</v>
+        <v>1027</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -6007,16 +6007,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1018</v>
+        <v>1028</v>
       </c>
       <c r="C7" s="2">
         <v>45612</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1039</v>
+        <v>1029</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -6049,16 +6049,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1019</v>
+        <v>1031</v>
       </c>
       <c r="C8" s="2">
         <v>45612</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1041</v>
+        <v>1032</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1042</v>
+        <v>1033</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -6091,16 +6091,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1020</v>
+        <v>1034</v>
       </c>
       <c r="C9" s="2">
         <v>45612</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1043</v>
+        <v>1035</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1044</v>
+        <v>1036</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -6133,13 +6133,13 @@
         <v>650</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1021</v>
+        <v>1037</v>
       </c>
       <c r="C10" s="2">
         <v>45612</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1045</v>
+        <v>1038</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
@@ -6173,16 +6173,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1022</v>
+        <v>1039</v>
       </c>
       <c r="C11" s="2">
         <v>45612</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1046</v>
+        <v>1040</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1047</v>
+        <v>1041</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -6215,13 +6215,13 @@
         <v>651</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1023</v>
+        <v>1042</v>
       </c>
       <c r="C12" s="2">
         <v>45613</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1">
@@ -6255,16 +6255,16 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1024</v>
+        <v>1044</v>
       </c>
       <c r="C13" s="2">
         <v>45613</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -6297,16 +6297,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1025</v>
+        <v>1047</v>
       </c>
       <c r="C14" s="2">
         <v>45619</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -6339,16 +6339,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1026</v>
+        <v>1050</v>
       </c>
       <c r="C15" s="2">
         <v>45619</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -6381,16 +6381,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1027</v>
+        <v>1053</v>
       </c>
       <c r="C16" s="2">
         <v>45620</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>1055</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>1056</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -6423,7 +6423,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1028</v>
+        <v>1056</v>
       </c>
       <c r="C17" s="2">
         <v>45620</v>

</xml_diff>